<commit_message>
fix bug in vibration off time
</commit_message>
<xml_diff>
--- a/Trials.xlsx
+++ b/Trials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PMDLAB\Documents\Python-Experiments\Vibration-targeting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3A79BB-978F-4956-9309-E9DE99104075}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FAEF51-161D-4724-AD57-9C9D6D7B2E46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="trial-randomizer" sheetId="7" r:id="rId1"/>
@@ -535,7 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAED357-3816-4D39-B84F-5153F27D449A}">
   <dimension ref="B2:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -677,8 +677,8 @@
         <v>3</v>
       </c>
       <c r="D21">
-        <f ca="1">RAND()</f>
-        <v>3.508223901441021E-2</v>
+        <f t="shared" ref="D21:D36" ca="1" si="0">RAND()</f>
+        <v>0.33000403608551854</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
@@ -689,8 +689,8 @@
         <v>3</v>
       </c>
       <c r="D22">
-        <f ca="1">RAND()</f>
-        <v>0.43102026259885295</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.47223313897931385</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
@@ -701,8 +701,8 @@
         <v>1</v>
       </c>
       <c r="D23">
-        <f ca="1">RAND()</f>
-        <v>0.14443544239351669</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.89416132333280685</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -713,8 +713,8 @@
         <v>1</v>
       </c>
       <c r="D24">
-        <f ca="1">RAND()</f>
-        <v>0.1288859155447053</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.39049068351369343</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -725,8 +725,8 @@
         <v>2</v>
       </c>
       <c r="D25">
-        <f ca="1">RAND()</f>
-        <v>0.6553150738216893</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.70283948166184662</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -737,8 +737,8 @@
         <v>2</v>
       </c>
       <c r="D26">
-        <f ca="1">RAND()</f>
-        <v>0.46792531755523836</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.90564428817636089</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -749,8 +749,8 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <f ca="1">RAND()</f>
-        <v>0.59150377058143933</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.82484752720354737</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -761,8 +761,8 @@
         <v>1</v>
       </c>
       <c r="D28">
-        <f ca="1">RAND()</f>
-        <v>0.34309023409666761</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.7972225350940626</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
@@ -773,8 +773,8 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <f ca="1">RAND()</f>
-        <v>1.7703693703573276E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.57989815612290718</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
@@ -785,8 +785,8 @@
         <v>3</v>
       </c>
       <c r="D30">
-        <f ca="1">RAND()</f>
-        <v>0.48666976131788564</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.79075733454041075</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
@@ -797,8 +797,8 @@
         <v>1</v>
       </c>
       <c r="D31">
-        <f ca="1">RAND()</f>
-        <v>9.7499552361893893E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.26582603891013745</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
@@ -809,8 +809,8 @@
         <v>0</v>
       </c>
       <c r="D32">
-        <f ca="1">RAND()</f>
-        <v>0.78951459901991983</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.21658644301855456</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
@@ -821,8 +821,8 @@
         <v>2</v>
       </c>
       <c r="D33">
-        <f ca="1">RAND()</f>
-        <v>0.94478999378846662</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.75481433021217581</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
@@ -833,8 +833,8 @@
         <v>3</v>
       </c>
       <c r="D34">
-        <f ca="1">RAND()</f>
-        <v>0.85073631269604466</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>8.3438951767883185E-2</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
@@ -845,8 +845,8 @@
         <v>2</v>
       </c>
       <c r="D35">
-        <f ca="1">RAND()</f>
-        <v>0.17769023260274996</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.6149211290699832</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
@@ -857,8 +857,8 @@
         <v>0</v>
       </c>
       <c r="D36">
-        <f ca="1">RAND()</f>
-        <v>0.55339215213333093</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.56034159082828483</v>
       </c>
     </row>
   </sheetData>
@@ -1056,10 +1056,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L81"/>
+  <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="N87" sqref="N87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,10 +1126,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -1164,10 +1164,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -1202,10 +1202,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -1240,10 +1240,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -1278,10 +1278,10 @@
         <v>3</v>
       </c>
       <c r="D6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -1316,10 +1316,10 @@
         <v>3</v>
       </c>
       <c r="D7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
@@ -1354,10 +1354,10 @@
         <v>3</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
@@ -1392,10 +1392,10 @@
         <v>3</v>
       </c>
       <c r="D9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
@@ -1430,10 +1430,10 @@
         <v>3</v>
       </c>
       <c r="D10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -1468,10 +1468,10 @@
         <v>3</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -1506,10 +1506,10 @@
         <v>3</v>
       </c>
       <c r="D12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -1544,10 +1544,10 @@
         <v>3</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -1582,10 +1582,10 @@
         <v>3</v>
       </c>
       <c r="D14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
@@ -1620,10 +1620,10 @@
         <v>3</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -1658,10 +1658,10 @@
         <v>3</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -1696,10 +1696,10 @@
         <v>3</v>
       </c>
       <c r="D17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -1728,7 +1728,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="C18" s="1">
         <v>3</v>
@@ -1755,7 +1755,7 @@
         <v>30</v>
       </c>
       <c r="K18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18" s="12">
         <v>0</v>
@@ -1766,7 +1766,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="C19" s="1">
         <v>3</v>
@@ -1793,7 +1793,7 @@
         <v>30</v>
       </c>
       <c r="K19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L19" s="12">
         <v>0</v>
@@ -1804,7 +1804,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="C20" s="1">
         <v>3</v>
@@ -1831,7 +1831,7 @@
         <v>30</v>
       </c>
       <c r="K20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L20" s="12">
         <v>0</v>
@@ -1842,7 +1842,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="C21" s="1">
         <v>3</v>
@@ -1869,7 +1869,7 @@
         <v>30</v>
       </c>
       <c r="K21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21" s="12">
         <v>0</v>
@@ -1880,16 +1880,16 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="C22" s="1">
         <v>3</v>
       </c>
       <c r="D22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
@@ -1907,7 +1907,7 @@
         <v>30</v>
       </c>
       <c r="K22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L22" s="12">
         <v>0</v>
@@ -1918,16 +1918,16 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="C23" s="1">
         <v>3</v>
       </c>
       <c r="D23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
@@ -1945,7 +1945,7 @@
         <v>30</v>
       </c>
       <c r="K23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L23" s="12">
         <v>0</v>
@@ -1956,16 +1956,16 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>135</v>
+        <v>75</v>
       </c>
       <c r="C24" s="1">
         <v>3</v>
       </c>
       <c r="D24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
@@ -1994,16 +1994,16 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="C25" s="1">
         <v>3</v>
       </c>
       <c r="D25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="1">
         <v>0</v>
@@ -2021,7 +2021,7 @@
         <v>30</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25" s="12">
         <v>0</v>
@@ -2038,10 +2038,10 @@
         <v>3</v>
       </c>
       <c r="D26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -2059,7 +2059,7 @@
         <v>30</v>
       </c>
       <c r="K26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L26" s="12">
         <v>0</v>
@@ -2070,16 +2070,16 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>75</v>
+        <v>135</v>
       </c>
       <c r="C27" s="1">
         <v>3</v>
       </c>
       <c r="D27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -2097,7 +2097,7 @@
         <v>30</v>
       </c>
       <c r="K27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L27" s="12">
         <v>0</v>
@@ -2114,10 +2114,10 @@
         <v>3</v>
       </c>
       <c r="D28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -2135,7 +2135,7 @@
         <v>30</v>
       </c>
       <c r="K28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L28" s="12">
         <v>0</v>
@@ -2146,16 +2146,16 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="C29" s="1">
         <v>3</v>
       </c>
       <c r="D29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
@@ -2184,16 +2184,16 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="C30" s="1">
         <v>3</v>
       </c>
       <c r="D30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30" s="1">
         <v>0</v>
@@ -2211,7 +2211,7 @@
         <v>30</v>
       </c>
       <c r="K30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L30" s="12">
         <v>0</v>
@@ -2228,10 +2228,10 @@
         <v>3</v>
       </c>
       <c r="D31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" s="1">
         <v>0</v>
@@ -2249,7 +2249,7 @@
         <v>30</v>
       </c>
       <c r="K31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L31" s="12">
         <v>0</v>
@@ -2260,16 +2260,16 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="C32" s="1">
         <v>3</v>
       </c>
       <c r="D32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32" s="1">
         <v>0</v>
@@ -2287,7 +2287,7 @@
         <v>30</v>
       </c>
       <c r="K32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L32" s="12">
         <v>0</v>
@@ -2298,16 +2298,16 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="C33" s="1">
         <v>3</v>
       </c>
       <c r="D33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" s="1">
         <v>0</v>
@@ -2325,7 +2325,7 @@
         <v>30</v>
       </c>
       <c r="K33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L33" s="12">
         <v>0</v>
@@ -2336,16 +2336,16 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C34" s="1">
         <v>3</v>
       </c>
       <c r="D34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" s="1">
         <v>0</v>
@@ -2363,7 +2363,7 @@
         <v>30</v>
       </c>
       <c r="K34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L34" s="12">
         <v>0</v>
@@ -2374,16 +2374,16 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>135</v>
+        <v>75</v>
       </c>
       <c r="C35" s="1">
         <v>3</v>
       </c>
       <c r="D35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" s="1">
         <v>0</v>
@@ -2401,7 +2401,7 @@
         <v>30</v>
       </c>
       <c r="K35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L35" s="12">
         <v>0</v>
@@ -2412,16 +2412,16 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="C36" s="1">
         <v>3</v>
       </c>
       <c r="D36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" s="1">
         <v>0</v>
@@ -2439,7 +2439,7 @@
         <v>30</v>
       </c>
       <c r="K36">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L36" s="12">
         <v>0</v>
@@ -2450,16 +2450,16 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="C37" s="1">
         <v>3</v>
       </c>
       <c r="D37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37" s="1">
         <v>0</v>
@@ -2477,7 +2477,7 @@
         <v>30</v>
       </c>
       <c r="K37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L37" s="12">
         <v>0</v>
@@ -2488,7 +2488,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="C38" s="1">
         <v>3</v>
@@ -2515,7 +2515,7 @@
         <v>30</v>
       </c>
       <c r="K38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L38" s="12">
         <v>0</v>
@@ -2553,7 +2553,7 @@
         <v>30</v>
       </c>
       <c r="K39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L39" s="12">
         <v>0</v>
@@ -2591,7 +2591,7 @@
         <v>30</v>
       </c>
       <c r="K40">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L40" s="12">
         <v>0</v>
@@ -2602,7 +2602,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>75</v>
+        <v>135</v>
       </c>
       <c r="C41" s="1">
         <v>3</v>
@@ -2646,10 +2646,10 @@
         <v>3</v>
       </c>
       <c r="D42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" s="1">
         <v>0</v>
@@ -2667,7 +2667,7 @@
         <v>30</v>
       </c>
       <c r="K42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L42" s="12">
         <v>0</v>
@@ -2684,10 +2684,10 @@
         <v>3</v>
       </c>
       <c r="D43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43" s="1">
         <v>0</v>
@@ -2705,7 +2705,7 @@
         <v>30</v>
       </c>
       <c r="K43">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L43" s="12">
         <v>0</v>
@@ -2716,16 +2716,16 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="C44" s="1">
         <v>3</v>
       </c>
       <c r="D44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" s="1">
         <v>0</v>
@@ -2743,7 +2743,7 @@
         <v>30</v>
       </c>
       <c r="K44">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L44" s="12">
         <v>0</v>
@@ -2754,16 +2754,16 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="C45" s="1">
         <v>3</v>
       </c>
       <c r="D45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" s="1">
         <v>0</v>
@@ -2781,7 +2781,7 @@
         <v>30</v>
       </c>
       <c r="K45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L45" s="12">
         <v>0</v>
@@ -2792,16 +2792,16 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="C46" s="1">
         <v>3</v>
       </c>
       <c r="D46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46" s="1">
         <v>0</v>
@@ -2830,16 +2830,16 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="C47" s="1">
         <v>3</v>
       </c>
       <c r="D47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47" s="1">
         <v>0</v>
@@ -2857,7 +2857,7 @@
         <v>30</v>
       </c>
       <c r="K47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L47" s="12">
         <v>0</v>
@@ -2868,16 +2868,16 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="C48" s="1">
         <v>3</v>
       </c>
       <c r="D48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" s="1">
         <v>0</v>
@@ -2895,7 +2895,7 @@
         <v>30</v>
       </c>
       <c r="K48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L48" s="12">
         <v>0</v>
@@ -2906,16 +2906,16 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="C49" s="1">
         <v>3</v>
       </c>
       <c r="D49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" s="1">
         <v>0</v>
@@ -2933,7 +2933,7 @@
         <v>30</v>
       </c>
       <c r="K49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L49" s="12">
         <v>0</v>
@@ -2944,16 +2944,16 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="C50" s="1">
         <v>3</v>
       </c>
       <c r="D50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F50" s="1">
         <v>0</v>
@@ -2971,7 +2971,7 @@
         <v>30</v>
       </c>
       <c r="K50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L50" s="12">
         <v>0</v>
@@ -2982,16 +2982,16 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="C51" s="1">
         <v>3</v>
       </c>
       <c r="D51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51" s="1">
         <v>0</v>
@@ -3009,7 +3009,7 @@
         <v>30</v>
       </c>
       <c r="K51">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L51" s="12">
         <v>0</v>
@@ -3026,10 +3026,10 @@
         <v>3</v>
       </c>
       <c r="D52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F52" s="1">
         <v>0</v>
@@ -3047,7 +3047,7 @@
         <v>30</v>
       </c>
       <c r="K52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L52" s="12">
         <v>0</v>
@@ -3058,16 +3058,16 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="C53" s="1">
         <v>3</v>
       </c>
       <c r="D53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F53" s="1">
         <v>0</v>
@@ -3085,7 +3085,7 @@
         <v>30</v>
       </c>
       <c r="K53">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L53" s="12">
         <v>0</v>
@@ -3096,16 +3096,16 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>75</v>
+        <v>135</v>
       </c>
       <c r="C54" s="1">
         <v>3</v>
       </c>
       <c r="D54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F54" s="1">
         <v>0</v>
@@ -3134,16 +3134,16 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="C55" s="1">
         <v>3</v>
       </c>
       <c r="D55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55" s="1">
         <v>0</v>
@@ -3161,7 +3161,7 @@
         <v>30</v>
       </c>
       <c r="K55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L55" s="12">
         <v>0</v>
@@ -3172,16 +3172,16 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>135</v>
+        <v>75</v>
       </c>
       <c r="C56" s="1">
         <v>3</v>
       </c>
       <c r="D56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56" s="1">
         <v>0</v>
@@ -3199,7 +3199,7 @@
         <v>30</v>
       </c>
       <c r="K56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L56" s="12">
         <v>0</v>
@@ -3210,16 +3210,16 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="C57" s="1">
         <v>3</v>
       </c>
       <c r="D57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57" s="1">
         <v>0</v>
@@ -3237,7 +3237,7 @@
         <v>30</v>
       </c>
       <c r="K57">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L57" s="12">
         <v>0</v>
@@ -3248,7 +3248,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="C58" s="1">
         <v>3</v>
@@ -3275,7 +3275,7 @@
         <v>30</v>
       </c>
       <c r="K58">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L58" s="12">
         <v>0</v>
@@ -3324,7 +3324,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="C60" s="1">
         <v>3</v>
@@ -3351,7 +3351,7 @@
         <v>30</v>
       </c>
       <c r="K60">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L60" s="12">
         <v>0</v>
@@ -3362,7 +3362,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="C61" s="1">
         <v>3</v>
@@ -3400,16 +3400,16 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="C62" s="1">
         <v>3</v>
       </c>
       <c r="D62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F62" s="1">
         <v>0</v>
@@ -3427,7 +3427,7 @@
         <v>30</v>
       </c>
       <c r="K62">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L62" s="12">
         <v>0</v>
@@ -3444,10 +3444,10 @@
         <v>3</v>
       </c>
       <c r="D63" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F63" s="1">
         <v>0</v>
@@ -3465,7 +3465,7 @@
         <v>30</v>
       </c>
       <c r="K63">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L63" s="12">
         <v>0</v>
@@ -3476,16 +3476,16 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C64" s="1">
         <v>3</v>
       </c>
       <c r="D64" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F64" s="1">
         <v>0</v>
@@ -3503,7 +3503,7 @@
         <v>30</v>
       </c>
       <c r="K64">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L64" s="12">
         <v>0</v>
@@ -3514,16 +3514,16 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="C65" s="1">
         <v>3</v>
       </c>
       <c r="D65" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F65" s="1">
         <v>0</v>
@@ -3552,16 +3552,16 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="C66" s="1">
         <v>3</v>
       </c>
       <c r="D66" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F66" s="1">
         <v>0</v>
@@ -3579,7 +3579,7 @@
         <v>30</v>
       </c>
       <c r="K66">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L66" s="12">
         <v>0</v>
@@ -3590,16 +3590,16 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>135</v>
+        <v>75</v>
       </c>
       <c r="C67" s="1">
         <v>3</v>
       </c>
       <c r="D67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67" s="1">
         <v>0</v>
@@ -3617,7 +3617,7 @@
         <v>30</v>
       </c>
       <c r="K67">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L67" s="12">
         <v>0</v>
@@ -3628,16 +3628,16 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>75</v>
+        <v>135</v>
       </c>
       <c r="C68" s="1">
         <v>3</v>
       </c>
       <c r="D68" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F68" s="1">
         <v>0</v>
@@ -3655,7 +3655,7 @@
         <v>30</v>
       </c>
       <c r="K68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L68" s="12">
         <v>0</v>
@@ -3666,16 +3666,16 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="C69" s="1">
         <v>3</v>
       </c>
       <c r="D69" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F69" s="1">
         <v>0</v>
@@ -3693,7 +3693,7 @@
         <v>30</v>
       </c>
       <c r="K69">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L69" s="12">
         <v>0</v>
@@ -3704,16 +3704,16 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C70" s="1">
         <v>3</v>
       </c>
       <c r="D70" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F70" s="1">
         <v>0</v>
@@ -3731,7 +3731,7 @@
         <v>30</v>
       </c>
       <c r="K70">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L70" s="12">
         <v>0</v>
@@ -3742,16 +3742,16 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>135</v>
+        <v>75</v>
       </c>
       <c r="C71" s="1">
         <v>3</v>
       </c>
       <c r="D71" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F71" s="1">
         <v>0</v>
@@ -3769,7 +3769,7 @@
         <v>30</v>
       </c>
       <c r="K71">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L71" s="12">
         <v>0</v>
@@ -3780,16 +3780,16 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="C72" s="1">
         <v>3</v>
       </c>
       <c r="D72" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F72" s="1">
         <v>0</v>
@@ -3807,7 +3807,7 @@
         <v>30</v>
       </c>
       <c r="K72">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L72" s="12">
         <v>0</v>
@@ -3818,16 +3818,16 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C73" s="1">
         <v>3</v>
       </c>
       <c r="D73" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F73" s="1">
         <v>0</v>
@@ -3845,7 +3845,7 @@
         <v>30</v>
       </c>
       <c r="K73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L73" s="12">
         <v>0</v>
@@ -3856,16 +3856,16 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="C74" s="1">
         <v>3</v>
       </c>
       <c r="D74" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F74" s="1">
         <v>0</v>
@@ -3883,7 +3883,7 @@
         <v>30</v>
       </c>
       <c r="K74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L74" s="12">
         <v>0</v>
@@ -3894,16 +3894,16 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="C75" s="1">
         <v>3</v>
       </c>
       <c r="D75" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F75" s="1">
         <v>0</v>
@@ -3921,7 +3921,7 @@
         <v>30</v>
       </c>
       <c r="K75">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L75" s="12">
         <v>0</v>
@@ -3932,16 +3932,16 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="C76" s="1">
         <v>3</v>
       </c>
       <c r="D76" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F76" s="1">
         <v>0</v>
@@ -3959,7 +3959,7 @@
         <v>30</v>
       </c>
       <c r="K76">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L76" s="12">
         <v>0</v>
@@ -3970,16 +3970,16 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="C77" s="1">
         <v>3</v>
       </c>
       <c r="D77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77" s="1">
         <v>0</v>
@@ -3997,7 +3997,7 @@
         <v>30</v>
       </c>
       <c r="K77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L77" s="12">
         <v>0</v>
@@ -4008,7 +4008,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="C78" s="1">
         <v>3</v>
@@ -4035,7 +4035,7 @@
         <v>30</v>
       </c>
       <c r="K78">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L78" s="12">
         <v>0</v>
@@ -4046,7 +4046,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="C79" s="1">
         <v>3</v>
@@ -4073,7 +4073,7 @@
         <v>30</v>
       </c>
       <c r="K79">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L79" s="12">
         <v>0</v>
@@ -4111,7 +4111,7 @@
         <v>30</v>
       </c>
       <c r="K80">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L80" s="12">
         <v>0</v>
@@ -4152,6 +4152,614 @@
         <v>0</v>
       </c>
       <c r="L81" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>105</v>
+      </c>
+      <c r="C82" s="1">
+        <v>3</v>
+      </c>
+      <c r="D82" s="1">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82" s="1">
+        <v>0</v>
+      </c>
+      <c r="G82" s="1">
+        <v>0</v>
+      </c>
+      <c r="H82" s="1">
+        <v>0</v>
+      </c>
+      <c r="I82" s="1">
+        <v>0</v>
+      </c>
+      <c r="J82" s="1">
+        <v>30</v>
+      </c>
+      <c r="K82">
+        <v>3</v>
+      </c>
+      <c r="L82" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>135</v>
+      </c>
+      <c r="C83" s="1">
+        <v>3</v>
+      </c>
+      <c r="D83" s="1">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0</v>
+      </c>
+      <c r="G83" s="1">
+        <v>0</v>
+      </c>
+      <c r="H83" s="1">
+        <v>0</v>
+      </c>
+      <c r="I83" s="1">
+        <v>0</v>
+      </c>
+      <c r="J83" s="1">
+        <v>30</v>
+      </c>
+      <c r="K83">
+        <v>3</v>
+      </c>
+      <c r="L83" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>75</v>
+      </c>
+      <c r="C84" s="1">
+        <v>3</v>
+      </c>
+      <c r="D84" s="1">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84" s="1">
+        <v>0</v>
+      </c>
+      <c r="G84" s="1">
+        <v>0</v>
+      </c>
+      <c r="H84" s="1">
+        <v>0</v>
+      </c>
+      <c r="I84" s="1">
+        <v>0</v>
+      </c>
+      <c r="J84" s="1">
+        <v>30</v>
+      </c>
+      <c r="K84">
+        <v>1</v>
+      </c>
+      <c r="L84" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>105</v>
+      </c>
+      <c r="C85" s="1">
+        <v>3</v>
+      </c>
+      <c r="D85" s="1">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85" s="1">
+        <v>0</v>
+      </c>
+      <c r="G85" s="1">
+        <v>0</v>
+      </c>
+      <c r="H85" s="1">
+        <v>0</v>
+      </c>
+      <c r="I85" s="1">
+        <v>0</v>
+      </c>
+      <c r="J85" s="1">
+        <v>30</v>
+      </c>
+      <c r="K85">
+        <v>1</v>
+      </c>
+      <c r="L85" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>45</v>
+      </c>
+      <c r="C86" s="1">
+        <v>3</v>
+      </c>
+      <c r="D86" s="1">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86" s="1">
+        <v>0</v>
+      </c>
+      <c r="G86" s="1">
+        <v>0</v>
+      </c>
+      <c r="H86" s="1">
+        <v>0</v>
+      </c>
+      <c r="I86" s="1">
+        <v>0</v>
+      </c>
+      <c r="J86" s="1">
+        <v>30</v>
+      </c>
+      <c r="K86">
+        <v>2</v>
+      </c>
+      <c r="L86" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>135</v>
+      </c>
+      <c r="C87" s="1">
+        <v>3</v>
+      </c>
+      <c r="D87" s="1">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87" s="1">
+        <v>0</v>
+      </c>
+      <c r="G87" s="1">
+        <v>0</v>
+      </c>
+      <c r="H87" s="1">
+        <v>0</v>
+      </c>
+      <c r="I87" s="1">
+        <v>0</v>
+      </c>
+      <c r="J87" s="1">
+        <v>30</v>
+      </c>
+      <c r="K87">
+        <v>2</v>
+      </c>
+      <c r="L87" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>45</v>
+      </c>
+      <c r="C88" s="1">
+        <v>3</v>
+      </c>
+      <c r="D88" s="1">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88" s="1">
+        <v>0</v>
+      </c>
+      <c r="G88" s="1">
+        <v>0</v>
+      </c>
+      <c r="H88" s="1">
+        <v>0</v>
+      </c>
+      <c r="I88" s="1">
+        <v>0</v>
+      </c>
+      <c r="J88" s="1">
+        <v>30</v>
+      </c>
+      <c r="K88">
+        <v>0</v>
+      </c>
+      <c r="L88" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>45</v>
+      </c>
+      <c r="C89" s="1">
+        <v>3</v>
+      </c>
+      <c r="D89" s="1">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89" s="1">
+        <v>0</v>
+      </c>
+      <c r="G89" s="1">
+        <v>0</v>
+      </c>
+      <c r="H89" s="1">
+        <v>0</v>
+      </c>
+      <c r="I89" s="1">
+        <v>0</v>
+      </c>
+      <c r="J89" s="1">
+        <v>30</v>
+      </c>
+      <c r="K89">
+        <v>1</v>
+      </c>
+      <c r="L89" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>75</v>
+      </c>
+      <c r="C90" s="1">
+        <v>3</v>
+      </c>
+      <c r="D90" s="1">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90" s="1">
+        <v>0</v>
+      </c>
+      <c r="G90" s="1">
+        <v>0</v>
+      </c>
+      <c r="H90" s="1">
+        <v>0</v>
+      </c>
+      <c r="I90" s="1">
+        <v>0</v>
+      </c>
+      <c r="J90" s="1">
+        <v>30</v>
+      </c>
+      <c r="K90">
+        <v>0</v>
+      </c>
+      <c r="L90" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>75</v>
+      </c>
+      <c r="C91" s="1">
+        <v>3</v>
+      </c>
+      <c r="D91" s="1">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91" s="1">
+        <v>0</v>
+      </c>
+      <c r="G91" s="1">
+        <v>0</v>
+      </c>
+      <c r="H91" s="1">
+        <v>0</v>
+      </c>
+      <c r="I91" s="1">
+        <v>0</v>
+      </c>
+      <c r="J91" s="1">
+        <v>30</v>
+      </c>
+      <c r="K91">
+        <v>3</v>
+      </c>
+      <c r="L91" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>135</v>
+      </c>
+      <c r="C92" s="1">
+        <v>3</v>
+      </c>
+      <c r="D92" s="1">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92" s="1">
+        <v>0</v>
+      </c>
+      <c r="G92" s="1">
+        <v>0</v>
+      </c>
+      <c r="H92" s="1">
+        <v>0</v>
+      </c>
+      <c r="I92" s="1">
+        <v>0</v>
+      </c>
+      <c r="J92" s="1">
+        <v>30</v>
+      </c>
+      <c r="K92">
+        <v>1</v>
+      </c>
+      <c r="L92" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>105</v>
+      </c>
+      <c r="C93" s="1">
+        <v>3</v>
+      </c>
+      <c r="D93" s="1">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93" s="1">
+        <v>0</v>
+      </c>
+      <c r="G93" s="1">
+        <v>0</v>
+      </c>
+      <c r="H93" s="1">
+        <v>0</v>
+      </c>
+      <c r="I93" s="1">
+        <v>0</v>
+      </c>
+      <c r="J93" s="1">
+        <v>30</v>
+      </c>
+      <c r="K93">
+        <v>0</v>
+      </c>
+      <c r="L93" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>75</v>
+      </c>
+      <c r="C94" s="1">
+        <v>3</v>
+      </c>
+      <c r="D94" s="1">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94" s="1">
+        <v>0</v>
+      </c>
+      <c r="G94" s="1">
+        <v>0</v>
+      </c>
+      <c r="H94" s="1">
+        <v>0</v>
+      </c>
+      <c r="I94" s="1">
+        <v>0</v>
+      </c>
+      <c r="J94" s="1">
+        <v>30</v>
+      </c>
+      <c r="K94">
+        <v>2</v>
+      </c>
+      <c r="L94" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>45</v>
+      </c>
+      <c r="C95" s="1">
+        <v>3</v>
+      </c>
+      <c r="D95" s="1">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95" s="1">
+        <v>0</v>
+      </c>
+      <c r="G95" s="1">
+        <v>0</v>
+      </c>
+      <c r="H95" s="1">
+        <v>0</v>
+      </c>
+      <c r="I95" s="1">
+        <v>0</v>
+      </c>
+      <c r="J95" s="1">
+        <v>30</v>
+      </c>
+      <c r="K95">
+        <v>3</v>
+      </c>
+      <c r="L95" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>105</v>
+      </c>
+      <c r="C96" s="1">
+        <v>3</v>
+      </c>
+      <c r="D96" s="1">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96" s="1">
+        <v>0</v>
+      </c>
+      <c r="G96" s="1">
+        <v>0</v>
+      </c>
+      <c r="H96" s="1">
+        <v>0</v>
+      </c>
+      <c r="I96" s="1">
+        <v>0</v>
+      </c>
+      <c r="J96" s="1">
+        <v>30</v>
+      </c>
+      <c r="K96">
+        <v>2</v>
+      </c>
+      <c r="L96" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>135</v>
+      </c>
+      <c r="C97" s="1">
+        <v>3</v>
+      </c>
+      <c r="D97" s="1">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97" s="1">
+        <v>0</v>
+      </c>
+      <c r="G97" s="1">
+        <v>0</v>
+      </c>
+      <c r="H97" s="1">
+        <v>0</v>
+      </c>
+      <c r="I97" s="1">
+        <v>0</v>
+      </c>
+      <c r="J97" s="1">
+        <v>30</v>
+      </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
+      <c r="L97" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4165,10 +4773,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4228,8 +4836,8 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>90</v>
+      <c r="B2">
+        <v>45</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
@@ -4237,8 +4845,8 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="1">
-        <v>0</v>
+      <c r="E2">
+        <v>1</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -4253,9 +4861,9 @@
         <v>0</v>
       </c>
       <c r="J2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
+        <v>30</v>
+      </c>
+      <c r="K2">
         <v>0</v>
       </c>
       <c r="L2" s="12">
@@ -4266,8 +4874,8 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>0</v>
+      <c r="B3">
+        <v>105</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
@@ -4275,8 +4883,8 @@
       <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3" s="1">
-        <v>0</v>
+      <c r="E3">
+        <v>1</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -4291,9 +4899,9 @@
         <v>0</v>
       </c>
       <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
+        <v>30</v>
+      </c>
+      <c r="K3">
         <v>0</v>
       </c>
       <c r="L3" s="12">
@@ -4304,8 +4912,8 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>180</v>
+      <c r="B4">
+        <v>105</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -4313,8 +4921,8 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="1">
-        <v>0</v>
+      <c r="E4">
+        <v>1</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -4329,9 +4937,9 @@
         <v>0</v>
       </c>
       <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1">
+        <v>30</v>
+      </c>
+      <c r="K4">
         <v>0</v>
       </c>
       <c r="L4" s="12">
@@ -4342,8 +4950,8 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
-        <v>45</v>
+      <c r="B5">
+        <v>135</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -4351,8 +4959,8 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="1">
-        <v>0</v>
+      <c r="E5">
+        <v>1</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -4367,9 +4975,9 @@
         <v>0</v>
       </c>
       <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1">
+        <v>30</v>
+      </c>
+      <c r="K5">
         <v>0</v>
       </c>
       <c r="L5" s="12">
@@ -4380,8 +4988,8 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
-        <v>135</v>
+      <c r="B6">
+        <v>45</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
@@ -4389,8 +4997,8 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="1">
-        <v>0</v>
+      <c r="E6">
+        <v>1</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -4405,9 +5013,12 @@
         <v>0</v>
       </c>
       <c r="J6" s="1">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1">
+        <v>30</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4415,8 +5026,8 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
-        <v>90</v>
+      <c r="B7">
+        <v>105</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
@@ -4424,8 +5035,8 @@
       <c r="D7" s="1">
         <v>1</v>
       </c>
-      <c r="E7" s="1">
-        <v>0</v>
+      <c r="E7">
+        <v>1</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
@@ -4440,9 +5051,12 @@
         <v>0</v>
       </c>
       <c r="J7" s="1">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1">
+        <v>30</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4450,8 +5064,8 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
-        <v>110</v>
+      <c r="B8">
+        <v>45</v>
       </c>
       <c r="C8" s="1">
         <v>3</v>
@@ -4459,8 +5073,8 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="1">
-        <v>0</v>
+      <c r="E8">
+        <v>1</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
@@ -4475,9 +5089,12 @@
         <v>0</v>
       </c>
       <c r="J8" s="1">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1">
+        <v>30</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4485,8 +5102,8 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
-        <v>70</v>
+      <c r="B9">
+        <v>135</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
@@ -4494,8 +5111,8 @@
       <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="1">
-        <v>0</v>
+      <c r="E9">
+        <v>1</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
@@ -4510,9 +5127,12 @@
         <v>0</v>
       </c>
       <c r="J9" s="1">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1">
+        <v>30</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4520,8 +5140,8 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
-        <v>80</v>
+      <c r="B10">
+        <v>135</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
@@ -4529,8 +5149,8 @@
       <c r="D10" s="1">
         <v>1</v>
       </c>
-      <c r="E10" s="1">
-        <v>0</v>
+      <c r="E10">
+        <v>1</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -4545,9 +5165,12 @@
         <v>0</v>
       </c>
       <c r="J10" s="1">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1">
+        <v>30</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4555,8 +5178,8 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
-        <v>100</v>
+      <c r="B11">
+        <v>135</v>
       </c>
       <c r="C11" s="1">
         <v>3</v>
@@ -4564,8 +5187,8 @@
       <c r="D11" s="1">
         <v>1</v>
       </c>
-      <c r="E11" s="1">
-        <v>0</v>
+      <c r="E11">
+        <v>1</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -4580,9 +5203,240 @@
         <v>0</v>
       </c>
       <c r="J11" s="1">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1">
+        <v>30</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>75</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>30</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>75</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>30</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>45</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>30</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>105</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>30</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>75</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>30</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>75</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>30</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17" s="12">
         <v>0</v>
       </c>
     </row>

</xml_diff>